<commit_message>
Added FDA 503A indicator
</commit_message>
<xml_diff>
--- a/report/_book/data/facility_info.xlsx
+++ b/report/_book/data/facility_info.xlsx
@@ -5,25 +5,25 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mburns/Desktop/bookdown-minimal-master/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mburns/Desktop/FDA-503B/report/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFBF0B75-B7F8-B44C-85AE-67070CA522CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23EFB986-3148-0241-84FE-417EBB549276}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8280" yWindow="500" windowWidth="30120" windowHeight="20140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2540" yWindow="500" windowWidth="35860" windowHeight="20140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="facility_info" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">facility_info!$A$1:$K$64</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">facility_info!$A$1:$L$64</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="168">
   <si>
     <t>lon</t>
   </si>
@@ -521,6 +521,12 @@
   </si>
   <si>
     <t>Lowellville</t>
+  </si>
+  <si>
+    <t>503A</t>
+  </si>
+  <si>
+    <t>Y</t>
   </si>
 </sst>
 </file>
@@ -1363,11 +1369,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K64"/>
+  <dimension ref="A1:L64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L65" sqref="L65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1380,7 +1386,7 @@
     <col min="11" max="11" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -1414,8 +1420,11 @@
       <c r="K1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -1449,8 +1458,11 @@
       <c r="K2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -1484,8 +1496,11 @@
       <c r="K3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -1519,8 +1534,11 @@
       <c r="K4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L4" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -1554,8 +1572,11 @@
       <c r="K5" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -1589,8 +1610,11 @@
       <c r="K6" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L6" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>32</v>
       </c>
@@ -1624,8 +1648,11 @@
       <c r="K7" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>35</v>
       </c>
@@ -1659,8 +1686,11 @@
       <c r="K8" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>36</v>
       </c>
@@ -1694,8 +1724,11 @@
       <c r="K9" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>39</v>
       </c>
@@ -1729,8 +1762,11 @@
       <c r="K10" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>42</v>
       </c>
@@ -1764,8 +1800,11 @@
       <c r="K11" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>45</v>
       </c>
@@ -1799,8 +1838,11 @@
       <c r="K12" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>48</v>
       </c>
@@ -1834,8 +1876,11 @@
       <c r="K13" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>51</v>
       </c>
@@ -1869,8 +1914,11 @@
       <c r="K14" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>54</v>
       </c>
@@ -1904,8 +1952,11 @@
       <c r="K15" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>58</v>
       </c>
@@ -1939,8 +1990,11 @@
       <c r="K16" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L16" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>60</v>
       </c>
@@ -1974,8 +2028,11 @@
       <c r="K17" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>63</v>
       </c>
@@ -2009,8 +2066,11 @@
       <c r="K18" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L18" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>67</v>
       </c>
@@ -2044,8 +2104,11 @@
       <c r="K19" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L19" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>69</v>
       </c>
@@ -2079,8 +2142,11 @@
       <c r="K20" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L20" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>72</v>
       </c>
@@ -2114,8 +2180,11 @@
       <c r="K21" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L21" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>74</v>
       </c>
@@ -2149,8 +2218,11 @@
       <c r="K22" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L22" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>76</v>
       </c>
@@ -2184,8 +2256,11 @@
       <c r="K23" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L23" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>79</v>
       </c>
@@ -2219,8 +2294,11 @@
       <c r="K24" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L24" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>82</v>
       </c>
@@ -2254,8 +2332,11 @@
       <c r="K25" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L25" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>83</v>
       </c>
@@ -2289,8 +2370,11 @@
       <c r="K26" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L26" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>85</v>
       </c>
@@ -2324,8 +2408,11 @@
       <c r="K27" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L27" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>87</v>
       </c>
@@ -2359,8 +2446,11 @@
       <c r="K28" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L28" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>89</v>
       </c>
@@ -2394,8 +2484,11 @@
       <c r="K29" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L29" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>92</v>
       </c>
@@ -2429,8 +2522,11 @@
       <c r="K30" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L30" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>94</v>
       </c>
@@ -2464,8 +2560,11 @@
       <c r="K31" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L31" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>96</v>
       </c>
@@ -2499,8 +2598,11 @@
       <c r="K32" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L32" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>98</v>
       </c>
@@ -2534,8 +2636,11 @@
       <c r="K33" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L33" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>100</v>
       </c>
@@ -2569,8 +2674,11 @@
       <c r="K34" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L34" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>102</v>
       </c>
@@ -2604,8 +2712,11 @@
       <c r="K35" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L35" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>104</v>
       </c>
@@ -2639,8 +2750,11 @@
       <c r="K36" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L36" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>106</v>
       </c>
@@ -2674,8 +2788,11 @@
       <c r="K37" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L37" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>108</v>
       </c>
@@ -2709,8 +2826,11 @@
       <c r="K38" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L38" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>111</v>
       </c>
@@ -2744,8 +2864,11 @@
       <c r="K39" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L39" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>113</v>
       </c>
@@ -2779,8 +2902,11 @@
       <c r="K40" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L40" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>115</v>
       </c>
@@ -2814,8 +2940,11 @@
       <c r="K41" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L41" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>118</v>
       </c>
@@ -2849,8 +2978,11 @@
       <c r="K42" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L42" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>119</v>
       </c>
@@ -2884,8 +3016,11 @@
       <c r="K43" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L43" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>122</v>
       </c>
@@ -2919,8 +3054,11 @@
       <c r="K44" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L44" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>124</v>
       </c>
@@ -2954,8 +3092,11 @@
       <c r="K45" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L45" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>126</v>
       </c>
@@ -2989,8 +3130,11 @@
       <c r="K46" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L46" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>129</v>
       </c>
@@ -3024,8 +3168,11 @@
       <c r="K47" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L47" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>131</v>
       </c>
@@ -3059,8 +3206,11 @@
       <c r="K48" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L48" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>133</v>
       </c>
@@ -3094,8 +3244,11 @@
       <c r="K49" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L49" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>135</v>
       </c>
@@ -3129,8 +3282,11 @@
       <c r="K50" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L50" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>137</v>
       </c>
@@ -3164,8 +3320,11 @@
       <c r="K51" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L51" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>139</v>
       </c>
@@ -3199,8 +3358,11 @@
       <c r="K52" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L52" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>142</v>
       </c>
@@ -3234,8 +3396,11 @@
       <c r="K53" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L53" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>145</v>
       </c>
@@ -3269,8 +3434,11 @@
       <c r="K54" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L54" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>147</v>
       </c>
@@ -3304,8 +3472,11 @@
       <c r="K55" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L55" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>149</v>
       </c>
@@ -3339,8 +3510,11 @@
       <c r="K56" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L56" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>151</v>
       </c>
@@ -3374,8 +3548,11 @@
       <c r="K57" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L57" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>153</v>
       </c>
@@ -3409,8 +3586,11 @@
       <c r="K58" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L58" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>155</v>
       </c>
@@ -3444,8 +3624,11 @@
       <c r="K59" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L59" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>157</v>
       </c>
@@ -3479,8 +3662,11 @@
       <c r="K60" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L60" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>159</v>
       </c>
@@ -3514,8 +3700,11 @@
       <c r="K61" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L61" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>160</v>
       </c>
@@ -3549,8 +3738,11 @@
       <c r="K62" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L62" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>162</v>
       </c>
@@ -3584,8 +3776,11 @@
       <c r="K63" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L63" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>163</v>
       </c>
@@ -3619,9 +3814,12 @@
       <c r="K64" t="s">
         <v>28</v>
       </c>
+      <c r="L64" t="s">
+        <v>27</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K64" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:L64" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>